<commit_message>
include Liyunet comments on Oromiya
</commit_message>
<xml_diff>
--- a/data/0.reference/2.look_ups/Oromiya/kebeles_field.xlsx
+++ b/data/0.reference/2.look_ups/Oromiya/kebeles_field.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="265">
   <si>
     <t xml:space="preserve">Region</t>
   </si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">w/kocha</t>
   </si>
   <si>
-    <t xml:space="preserve">hetosa</t>
+    <t xml:space="preserve">hitosa</t>
   </si>
   <si>
     <t xml:space="preserve">daya debo</t>
@@ -236,12 +236,27 @@
     <t xml:space="preserve">bedeno</t>
   </si>
   <si>
+    <t xml:space="preserve">badannoo</t>
+  </si>
+  <si>
     <t xml:space="preserve">dheertu</t>
   </si>
   <si>
+    <t xml:space="preserve">dhertu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ganamii</t>
+  </si>
+  <si>
     <t xml:space="preserve">goramii</t>
   </si>
   <si>
+    <t xml:space="preserve">i/buna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t/mangudoo</t>
+  </si>
+  <si>
     <t xml:space="preserve">t/qalaa</t>
   </si>
   <si>
@@ -251,21 +266,51 @@
     <t xml:space="preserve">burqaa</t>
   </si>
   <si>
-    <t xml:space="preserve">fadiis</t>
+    <t xml:space="preserve">deder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h/quni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m/dadar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/g/sadii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yatuu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fedis</t>
   </si>
   <si>
     <t xml:space="preserve">badhaatuu</t>
   </si>
   <si>
+    <t xml:space="preserve">bedha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bidbare</t>
+  </si>
+  <si>
     <t xml:space="preserve">bidbora</t>
   </si>
   <si>
     <t xml:space="preserve">facatuu</t>
   </si>
   <si>
+    <t xml:space="preserve">kaboot</t>
+  </si>
+  <si>
     <t xml:space="preserve">mul’ata</t>
   </si>
   <si>
+    <t xml:space="preserve">mulat</t>
+  </si>
+  <si>
     <t xml:space="preserve">qarree</t>
   </si>
   <si>
@@ -317,12 +362,27 @@
     <t xml:space="preserve">gursum</t>
   </si>
   <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a/s/o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b/nagaya</t>
+  </si>
+  <si>
     <t xml:space="preserve">biyyo  nagaya</t>
   </si>
   <si>
     <t xml:space="preserve">daayifarsa</t>
   </si>
   <si>
+    <t xml:space="preserve">dayfars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fu/huji</t>
+  </si>
+  <si>
     <t xml:space="preserve">funya jubaa</t>
   </si>
   <si>
@@ -362,27 +422,42 @@
     <t xml:space="preserve">mulaata</t>
   </si>
   <si>
-    <t xml:space="preserve">meeta</t>
+    <t xml:space="preserve">meta</t>
   </si>
   <si>
     <t xml:space="preserve">calanqoo  01</t>
   </si>
   <si>
+    <t xml:space="preserve">cayol</t>
+  </si>
+  <si>
     <t xml:space="preserve">h /bilisumma</t>
   </si>
   <si>
+    <t xml:space="preserve">h/bity</t>
+  </si>
+  <si>
     <t xml:space="preserve">wayibar</t>
   </si>
   <si>
+    <t xml:space="preserve">wogbay</t>
+  </si>
+  <si>
     <t xml:space="preserve">midega tola</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <t xml:space="preserve">bilisumaa</t>
   </si>
   <si>
     <t xml:space="preserve">leencaa</t>
   </si>
   <si>
+    <t xml:space="preserve">m/balii</t>
+  </si>
+  <si>
     <t xml:space="preserve">mu/balaa</t>
   </si>
   <si>
@@ -494,96 +569,6 @@
     <t xml:space="preserve">wakto mulu</t>
   </si>
   <si>
-    <t xml:space="preserve">unkown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">badannoo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dhertu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ganamii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i/buna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t/mangudoo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dadar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">golu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h/quni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m/dadar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n/g/sadii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yatuu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fedis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bedha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bidbare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kaboot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mulat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gursuum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a/s/o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b/nagaya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dayfars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fu/huji</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m/tola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m/balii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cayol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h/bity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wogbay</t>
-  </si>
-  <si>
     <t xml:space="preserve">west arsi</t>
   </si>
   <si>
@@ -614,6 +599,21 @@
     <t xml:space="preserve">sh/ne</t>
   </si>
   <si>
+    <t xml:space="preserve">arsi negele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aliwayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b/reji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dashe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mararo</t>
+  </si>
+  <si>
     <t xml:space="preserve">arsii</t>
   </si>
   <si>
@@ -684,21 +684,6 @@
   </si>
   <si>
     <t xml:space="preserve">shifa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nagele</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aliwayo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b/reji</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dashe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mararo</t>
   </si>
   <si>
     <t xml:space="preserve">h/d</t>
@@ -2029,7 +2014,9 @@
       <c r="C63" t="s">
         <v>73</v>
       </c>
-      <c r="D63"/>
+      <c r="D63" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
@@ -2039,9 +2026,11 @@
         <v>72</v>
       </c>
       <c r="C64" t="s">
-        <v>78</v>
-      </c>
-      <c r="D64"/>
+        <v>73</v>
+      </c>
+      <c r="D64" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
@@ -2051,7 +2040,7 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D65" t="s">
         <v>80</v>
@@ -2065,7 +2054,7 @@
         <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D66" t="s">
         <v>81</v>
@@ -2079,7 +2068,7 @@
         <v>72</v>
       </c>
       <c r="C67" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D67" t="s">
         <v>82</v>
@@ -2093,11 +2082,9 @@
         <v>72</v>
       </c>
       <c r="C68" t="s">
-        <v>79</v>
-      </c>
-      <c r="D68" t="s">
-        <v>83</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
@@ -2107,11 +2094,9 @@
         <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
-      </c>
-      <c r="D69" t="s">
-        <v>84</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
@@ -2121,9 +2106,11 @@
         <v>72</v>
       </c>
       <c r="C70" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70" t="s">
         <v>85</v>
       </c>
-      <c r="D70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
@@ -2133,10 +2120,10 @@
         <v>72</v>
       </c>
       <c r="C71" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" t="s">
         <v>86</v>
-      </c>
-      <c r="D71" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="72">
@@ -2147,10 +2134,10 @@
         <v>72</v>
       </c>
       <c r="C72" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73">
@@ -2161,9 +2148,11 @@
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>86</v>
-      </c>
-      <c r="D73"/>
+        <v>84</v>
+      </c>
+      <c r="D73" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
@@ -2173,10 +2162,10 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
+        <v>84</v>
+      </c>
+      <c r="D74" t="s">
         <v>89</v>
-      </c>
-      <c r="D74" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="75">
@@ -2187,7 +2176,7 @@
         <v>72</v>
       </c>
       <c r="C75" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D75" t="s">
         <v>91</v>
@@ -2201,7 +2190,7 @@
         <v>72</v>
       </c>
       <c r="C76" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D76" t="s">
         <v>92</v>
@@ -2215,7 +2204,7 @@
         <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D77" t="s">
         <v>93</v>
@@ -2229,7 +2218,7 @@
         <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D78" t="s">
         <v>94</v>
@@ -2243,10 +2232,10 @@
         <v>72</v>
       </c>
       <c r="C79" t="s">
+        <v>90</v>
+      </c>
+      <c r="D79" t="s">
         <v>95</v>
-      </c>
-      <c r="D79" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="80">
@@ -2257,10 +2246,10 @@
         <v>72</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D80" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81">
@@ -2271,10 +2260,10 @@
         <v>72</v>
       </c>
       <c r="C81" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82">
@@ -2285,9 +2274,11 @@
         <v>72</v>
       </c>
       <c r="C82" t="s">
-        <v>99</v>
-      </c>
-      <c r="D82"/>
+        <v>90</v>
+      </c>
+      <c r="D82" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
@@ -2297,10 +2288,10 @@
         <v>72</v>
       </c>
       <c r="C83" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D83" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84">
@@ -2311,11 +2302,9 @@
         <v>72</v>
       </c>
       <c r="C84" t="s">
-        <v>100</v>
-      </c>
-      <c r="D84" t="s">
-        <v>102</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D84"/>
     </row>
     <row r="85">
       <c r="A85" t="s">
@@ -2327,9 +2316,7 @@
       <c r="C85" t="s">
         <v>100</v>
       </c>
-      <c r="D85" t="s">
-        <v>103</v>
-      </c>
+      <c r="D85"/>
     </row>
     <row r="86">
       <c r="A86" t="s">
@@ -2339,10 +2326,10 @@
         <v>72</v>
       </c>
       <c r="C86" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D86" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87">
@@ -2353,10 +2340,10 @@
         <v>72</v>
       </c>
       <c r="C87" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D87" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88">
@@ -2367,11 +2354,9 @@
         <v>72</v>
       </c>
       <c r="C88" t="s">
-        <v>105</v>
-      </c>
-      <c r="D88" t="s">
-        <v>107</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D88"/>
     </row>
     <row r="89">
       <c r="A89" t="s">
@@ -2381,10 +2366,10 @@
         <v>72</v>
       </c>
       <c r="C89" t="s">
+        <v>104</v>
+      </c>
+      <c r="D89" t="s">
         <v>105</v>
-      </c>
-      <c r="D89" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="90">
@@ -2395,10 +2380,10 @@
         <v>72</v>
       </c>
       <c r="C90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D90" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91">
@@ -2409,10 +2394,10 @@
         <v>72</v>
       </c>
       <c r="C91" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D91" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92">
@@ -2423,10 +2408,10 @@
         <v>72</v>
       </c>
       <c r="C92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D92" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93">
@@ -2437,10 +2422,10 @@
         <v>72</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D93" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94">
@@ -2451,10 +2436,10 @@
         <v>72</v>
       </c>
       <c r="C94" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D94" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95">
@@ -2465,9 +2450,11 @@
         <v>72</v>
       </c>
       <c r="C95" t="s">
-        <v>105</v>
-      </c>
-      <c r="D95"/>
+        <v>110</v>
+      </c>
+      <c r="D95" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
@@ -2477,10 +2464,10 @@
         <v>72</v>
       </c>
       <c r="C96" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D96" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97">
@@ -2491,11 +2478,9 @@
         <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>116</v>
-      </c>
-      <c r="D97" t="s">
-        <v>117</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D97"/>
     </row>
     <row r="98">
       <c r="A98" t="s">
@@ -2505,10 +2490,10 @@
         <v>72</v>
       </c>
       <c r="C98" t="s">
+        <v>115</v>
+      </c>
+      <c r="D98" t="s">
         <v>116</v>
-      </c>
-      <c r="D98" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="99">
@@ -2519,10 +2504,10 @@
         <v>72</v>
       </c>
       <c r="C99" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D99" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100">
@@ -2533,10 +2518,10 @@
         <v>72</v>
       </c>
       <c r="C100" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D100" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="101">
@@ -2547,10 +2532,10 @@
         <v>72</v>
       </c>
       <c r="C101" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D101" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102">
@@ -2561,10 +2546,10 @@
         <v>72</v>
       </c>
       <c r="C102" t="s">
+        <v>115</v>
+      </c>
+      <c r="D102" t="s">
         <v>120</v>
-      </c>
-      <c r="D102" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="103">
@@ -2575,10 +2560,10 @@
         <v>72</v>
       </c>
       <c r="C103" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D103" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104">
@@ -2589,9 +2574,11 @@
         <v>72</v>
       </c>
       <c r="C104" t="s">
-        <v>120</v>
-      </c>
-      <c r="D104"/>
+        <v>115</v>
+      </c>
+      <c r="D104" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
@@ -2601,10 +2588,10 @@
         <v>72</v>
       </c>
       <c r="C105" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D105" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="106">
@@ -2615,10 +2602,10 @@
         <v>72</v>
       </c>
       <c r="C106" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D106" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="107">
@@ -2626,13 +2613,13 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C107" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D107" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108">
@@ -2640,13 +2627,13 @@
         <v>4</v>
       </c>
       <c r="B108" t="s">
+        <v>72</v>
+      </c>
+      <c r="C108" t="s">
+        <v>125</v>
+      </c>
+      <c r="D108" t="s">
         <v>127</v>
-      </c>
-      <c r="C108" t="s">
-        <v>128</v>
-      </c>
-      <c r="D108" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="109">
@@ -2654,13 +2641,13 @@
         <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C109" t="s">
+        <v>125</v>
+      </c>
+      <c r="D109" t="s">
         <v>128</v>
-      </c>
-      <c r="D109" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="110">
@@ -2668,13 +2655,13 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C110" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D110" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="111">
@@ -2682,13 +2669,13 @@
         <v>4</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C111" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D111" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112">
@@ -2696,13 +2683,13 @@
         <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C112" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D112" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="113">
@@ -2710,13 +2697,13 @@
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C113" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D113" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="114">
@@ -2724,13 +2711,13 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C114" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D114" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="115">
@@ -2738,27 +2725,25 @@
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C115" t="s">
-        <v>128</v>
-      </c>
-      <c r="D115" t="s">
-        <v>137</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D115"/>
     </row>
     <row r="116">
       <c r="A116" t="s">
         <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C116" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D116" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="117">
@@ -2766,25 +2751,27 @@
         <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C117" t="s">
-        <v>139</v>
-      </c>
-      <c r="D117"/>
+        <v>136</v>
+      </c>
+      <c r="D117" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
         <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C118" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D118" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119">
@@ -2792,13 +2779,13 @@
         <v>4</v>
       </c>
       <c r="B119" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C119" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D119" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120">
@@ -2806,13 +2793,13 @@
         <v>4</v>
       </c>
       <c r="B120" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C120" t="s">
+        <v>136</v>
+      </c>
+      <c r="D120" t="s">
         <v>140</v>
-      </c>
-      <c r="D120" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="121">
@@ -2820,13 +2807,13 @@
         <v>4</v>
       </c>
       <c r="B121" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C121" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D121" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="122">
@@ -2834,39 +2821,39 @@
         <v>4</v>
       </c>
       <c r="B122" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C122" t="s">
-        <v>145</v>
-      </c>
-      <c r="D122"/>
+        <v>136</v>
+      </c>
+      <c r="D122" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
         <v>4</v>
       </c>
       <c r="B123" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C123" t="s">
-        <v>146</v>
-      </c>
-      <c r="D123" t="s">
-        <v>147</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D123"/>
     </row>
     <row r="124">
       <c r="A124" t="s">
         <v>4</v>
       </c>
       <c r="B124" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C124" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D124" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125">
@@ -2874,13 +2861,13 @@
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C125" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D125" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="126">
@@ -2888,13 +2875,13 @@
         <v>4</v>
       </c>
       <c r="B126" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C126" t="s">
+        <v>143</v>
+      </c>
+      <c r="D126" t="s">
         <v>146</v>
-      </c>
-      <c r="D126" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="127">
@@ -2902,13 +2889,13 @@
         <v>4</v>
       </c>
       <c r="B127" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C127" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D127" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="128">
@@ -2916,13 +2903,13 @@
         <v>4</v>
       </c>
       <c r="B128" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C128" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D128" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="129">
@@ -2930,13 +2917,13 @@
         <v>4</v>
       </c>
       <c r="B129" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C129" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D129" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="130">
@@ -2944,27 +2931,25 @@
         <v>4</v>
       </c>
       <c r="B130" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C130" t="s">
-        <v>146</v>
-      </c>
-      <c r="D130" t="s">
-        <v>154</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D130"/>
     </row>
     <row r="131">
       <c r="A131" t="s">
         <v>4</v>
       </c>
       <c r="B131" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C131" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D131" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="132">
@@ -2972,13 +2957,13 @@
         <v>4</v>
       </c>
       <c r="B132" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C132" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D132" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="133">
@@ -2986,13 +2971,13 @@
         <v>4</v>
       </c>
       <c r="B133" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C133" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D133" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="134">
@@ -3000,13 +2985,13 @@
         <v>4</v>
       </c>
       <c r="B134" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C134" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D134" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135">
@@ -3014,13 +2999,13 @@
         <v>4</v>
       </c>
       <c r="B135" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C135" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D135" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="136">
@@ -3028,13 +3013,13 @@
         <v>4</v>
       </c>
       <c r="B136" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C136" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D136" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137">
@@ -3042,13 +3027,13 @@
         <v>4</v>
       </c>
       <c r="B137" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C137" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D137" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138">
@@ -3056,13 +3041,13 @@
         <v>4</v>
       </c>
       <c r="B138" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C138" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D138" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="139">
@@ -3070,13 +3055,13 @@
         <v>4</v>
       </c>
       <c r="B139" t="s">
+        <v>152</v>
+      </c>
+      <c r="C139" t="s">
+        <v>153</v>
+      </c>
+      <c r="D139" t="s">
         <v>160</v>
-      </c>
-      <c r="C139" t="s">
-        <v>73</v>
-      </c>
-      <c r="D139" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="140">
@@ -3084,13 +3069,13 @@
         <v>4</v>
       </c>
       <c r="B140" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C140" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D140" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="141">
@@ -3098,13 +3083,13 @@
         <v>4</v>
       </c>
       <c r="B141" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C141" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D141" t="s">
-        <v>76</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142">
@@ -3112,13 +3097,13 @@
         <v>4</v>
       </c>
       <c r="B142" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C142" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="D142" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="143">
@@ -3126,27 +3111,25 @@
         <v>4</v>
       </c>
       <c r="B143" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C143" t="s">
-        <v>166</v>
-      </c>
-      <c r="D143" t="s">
-        <v>168</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="D143"/>
     </row>
     <row r="144">
       <c r="A144" t="s">
         <v>4</v>
       </c>
       <c r="B144" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C144" t="s">
+        <v>165</v>
+      </c>
+      <c r="D144" t="s">
         <v>166</v>
-      </c>
-      <c r="D144" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="145">
@@ -3154,13 +3137,13 @@
         <v>4</v>
       </c>
       <c r="B145" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C145" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D145" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="146">
@@ -3168,13 +3151,13 @@
         <v>4</v>
       </c>
       <c r="B146" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C146" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D146" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="147">
@@ -3182,13 +3165,13 @@
         <v>4</v>
       </c>
       <c r="B147" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C147" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D147" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="148">
@@ -3196,27 +3179,25 @@
         <v>4</v>
       </c>
       <c r="B148" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C148" t="s">
-        <v>172</v>
-      </c>
-      <c r="D148" t="s">
-        <v>174</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D148"/>
     </row>
     <row r="149">
       <c r="A149" t="s">
         <v>4</v>
       </c>
       <c r="B149" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C149" t="s">
+        <v>171</v>
+      </c>
+      <c r="D149" t="s">
         <v>172</v>
-      </c>
-      <c r="D149" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="150">
@@ -3224,13 +3205,13 @@
         <v>4</v>
       </c>
       <c r="B150" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C150" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D150" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="151">
@@ -3238,25 +3219,27 @@
         <v>4</v>
       </c>
       <c r="B151" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C151" t="s">
-        <v>172</v>
-      </c>
-      <c r="D151"/>
+        <v>171</v>
+      </c>
+      <c r="D151" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
         <v>4</v>
       </c>
       <c r="B152" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C152" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D152" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="153">
@@ -3264,13 +3247,13 @@
         <v>4</v>
       </c>
       <c r="B153" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C153" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D153" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154">
@@ -3278,13 +3261,13 @@
         <v>4</v>
       </c>
       <c r="B154" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C154" t="s">
+        <v>171</v>
+      </c>
+      <c r="D154" t="s">
         <v>177</v>
-      </c>
-      <c r="D154" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="155">
@@ -3292,13 +3275,13 @@
         <v>4</v>
       </c>
       <c r="B155" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C155" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D155" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="156">
@@ -3306,13 +3289,13 @@
         <v>4</v>
       </c>
       <c r="B156" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C156" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D156" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="157">
@@ -3320,13 +3303,13 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C157" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D157" t="s">
-        <v>104</v>
+        <v>180</v>
       </c>
     </row>
     <row r="158">
@@ -3334,13 +3317,13 @@
         <v>4</v>
       </c>
       <c r="B158" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C158" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D158" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="159">
@@ -3348,13 +3331,13 @@
         <v>4</v>
       </c>
       <c r="B159" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C159" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D159" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
     </row>
     <row r="160">
@@ -3362,13 +3345,13 @@
         <v>4</v>
       </c>
       <c r="B160" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C160" t="s">
+        <v>171</v>
+      </c>
+      <c r="D160" t="s">
         <v>183</v>
-      </c>
-      <c r="D160" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="161">
@@ -3376,13 +3359,13 @@
         <v>4</v>
       </c>
       <c r="B161" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C161" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D161" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="162">
@@ -3390,13 +3373,13 @@
         <v>4</v>
       </c>
       <c r="B162" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="C162" t="s">
         <v>186</v>
       </c>
       <c r="D162" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
     </row>
     <row r="163">
@@ -3404,13 +3387,13 @@
         <v>4</v>
       </c>
       <c r="B163" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="C163" t="s">
         <v>186</v>
       </c>
       <c r="D163" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="164">
@@ -3418,35 +3401,41 @@
         <v>4</v>
       </c>
       <c r="B164" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="C164" t="s">
         <v>186</v>
       </c>
-      <c r="D164"/>
+      <c r="D164" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
         <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>160</v>
-      </c>
-      <c r="C165"/>
-      <c r="D165"/>
+        <v>185</v>
+      </c>
+      <c r="C165" t="s">
+        <v>186</v>
+      </c>
+      <c r="D165" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
         <v>4</v>
       </c>
       <c r="B166" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C166" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D166" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
     </row>
     <row r="167">
@@ -3454,13 +3443,13 @@
         <v>4</v>
       </c>
       <c r="B167" t="s">
+        <v>185</v>
+      </c>
+      <c r="C167" t="s">
+        <v>186</v>
+      </c>
+      <c r="D167" t="s">
         <v>190</v>
-      </c>
-      <c r="C167" t="s">
-        <v>191</v>
-      </c>
-      <c r="D167" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="168">
@@ -3468,13 +3457,13 @@
         <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C168" t="s">
         <v>191</v>
       </c>
       <c r="D168" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="169">
@@ -3482,13 +3471,13 @@
         <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C169" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D169" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
     </row>
     <row r="170">
@@ -3496,13 +3485,13 @@
         <v>4</v>
       </c>
       <c r="B170" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C170" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D170" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
     </row>
     <row r="171">
@@ -3510,13 +3499,13 @@
         <v>4</v>
       </c>
       <c r="B171" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C171" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D171" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="172">
@@ -3524,10 +3513,10 @@
         <v>4</v>
       </c>
       <c r="B172" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C172" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D172" t="s">
         <v>197</v>
@@ -3538,13 +3527,13 @@
         <v>4</v>
       </c>
       <c r="B173" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C173" t="s">
+        <v>195</v>
+      </c>
+      <c r="D173" t="s">
         <v>198</v>
-      </c>
-      <c r="D173" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="174">
@@ -3552,10 +3541,10 @@
         <v>4</v>
       </c>
       <c r="B174" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C174" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D174" t="s">
         <v>199</v>
@@ -3566,10 +3555,10 @@
         <v>4</v>
       </c>
       <c r="B175" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C175" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D175"/>
     </row>
@@ -3578,27 +3567,25 @@
         <v>4</v>
       </c>
       <c r="B176" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C176" t="s">
-        <v>201</v>
-      </c>
-      <c r="D176" t="s">
-        <v>202</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D176"/>
     </row>
     <row r="177">
       <c r="A177" t="s">
         <v>4</v>
       </c>
       <c r="B177" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C177" t="s">
         <v>201</v>
       </c>
       <c r="D177" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="178">
@@ -3606,13 +3593,13 @@
         <v>4</v>
       </c>
       <c r="B178" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C178" t="s">
         <v>201</v>
       </c>
       <c r="D178" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="179">
@@ -3620,13 +3607,13 @@
         <v>4</v>
       </c>
       <c r="B179" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C179" t="s">
-        <v>17</v>
+        <v>201</v>
       </c>
       <c r="D179" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="180">
@@ -3634,13 +3621,13 @@
         <v>4</v>
       </c>
       <c r="B180" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C180" t="s">
         <v>17</v>
       </c>
       <c r="D180" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="181">
@@ -3648,13 +3635,13 @@
         <v>4</v>
       </c>
       <c r="B181" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C181" t="s">
         <v>17</v>
       </c>
       <c r="D181" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="182">
@@ -3662,13 +3649,13 @@
         <v>4</v>
       </c>
       <c r="B182" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C182" t="s">
-        <v>207</v>
+        <v>17</v>
       </c>
       <c r="D182" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="183">
@@ -3676,13 +3663,13 @@
         <v>4</v>
       </c>
       <c r="B183" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C183" t="s">
         <v>207</v>
       </c>
       <c r="D183" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="184">
@@ -3690,13 +3677,13 @@
         <v>4</v>
       </c>
       <c r="B184" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C184" t="s">
         <v>207</v>
       </c>
       <c r="D184" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="185">
@@ -3704,13 +3691,13 @@
         <v>4</v>
       </c>
       <c r="B185" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C185" t="s">
         <v>207</v>
       </c>
       <c r="D185" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="186">
@@ -3718,13 +3705,13 @@
         <v>4</v>
       </c>
       <c r="B186" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C186" t="s">
         <v>207</v>
       </c>
       <c r="D186" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="187">
@@ -3732,13 +3719,13 @@
         <v>4</v>
       </c>
       <c r="B187" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C187" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D187" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="188">
@@ -3746,13 +3733,13 @@
         <v>4</v>
       </c>
       <c r="B188" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C188" t="s">
         <v>213</v>
       </c>
       <c r="D188" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="189">
@@ -3760,13 +3747,13 @@
         <v>4</v>
       </c>
       <c r="B189" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C189" t="s">
         <v>213</v>
       </c>
       <c r="D189" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="190">
@@ -3774,13 +3761,13 @@
         <v>4</v>
       </c>
       <c r="B190" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C190" t="s">
         <v>213</v>
       </c>
       <c r="D190" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="191">
@@ -3788,13 +3775,13 @@
         <v>4</v>
       </c>
       <c r="B191" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C191" t="s">
         <v>213</v>
       </c>
       <c r="D191" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="192">
@@ -3802,13 +3789,13 @@
         <v>4</v>
       </c>
       <c r="B192" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C192" t="s">
         <v>213</v>
       </c>
       <c r="D192" t="s">
-        <v>152</v>
+        <v>218</v>
       </c>
     </row>
     <row r="193">
@@ -3816,13 +3803,13 @@
         <v>4</v>
       </c>
       <c r="B193" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C193" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D193" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
     </row>
     <row r="194">
@@ -3830,13 +3817,13 @@
         <v>4</v>
       </c>
       <c r="B194" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C194" t="s">
         <v>219</v>
       </c>
       <c r="D194" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="195">
@@ -3844,13 +3831,13 @@
         <v>4</v>
       </c>
       <c r="B195" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C195" t="s">
         <v>219</v>
       </c>
       <c r="D195" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="196">
@@ -3858,13 +3845,13 @@
         <v>4</v>
       </c>
       <c r="B196" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C196" t="s">
         <v>219</v>
       </c>
       <c r="D196" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="197">
@@ -3872,13 +3859,13 @@
         <v>4</v>
       </c>
       <c r="B197" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C197" t="s">
         <v>219</v>
       </c>
       <c r="D197" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="198">
@@ -3886,13 +3873,13 @@
         <v>4</v>
       </c>
       <c r="B198" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C198" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D198" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="199">
@@ -3900,13 +3887,13 @@
         <v>4</v>
       </c>
       <c r="B199" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C199" t="s">
+        <v>21</v>
+      </c>
+      <c r="D199" t="s">
         <v>224</v>
-      </c>
-      <c r="D199" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="200">
@@ -3914,13 +3901,13 @@
         <v>4</v>
       </c>
       <c r="B200" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C200" t="s">
-        <v>224</v>
+        <v>21</v>
       </c>
       <c r="D200" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="201">
@@ -3928,13 +3915,13 @@
         <v>4</v>
       </c>
       <c r="B201" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C201" t="s">
-        <v>224</v>
+        <v>21</v>
       </c>
       <c r="D201" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="202">
@@ -3942,10 +3929,10 @@
         <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C202" t="s">
-        <v>224</v>
+        <v>21</v>
       </c>
       <c r="D202"/>
     </row>
@@ -3954,13 +3941,13 @@
         <v>4</v>
       </c>
       <c r="B203" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C203" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D203" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="204">
@@ -3968,13 +3955,13 @@
         <v>4</v>
       </c>
       <c r="B204" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C204" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D204" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="205">
@@ -3982,13 +3969,13 @@
         <v>4</v>
       </c>
       <c r="B205" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C205" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D205" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="206">
@@ -3996,25 +3983,27 @@
         <v>4</v>
       </c>
       <c r="B206" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C206" t="s">
-        <v>21</v>
-      </c>
-      <c r="D206"/>
+        <v>25</v>
+      </c>
+      <c r="D206" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
         <v>4</v>
       </c>
       <c r="B207" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C207" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D207" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="208">
@@ -4022,13 +4011,13 @@
         <v>4</v>
       </c>
       <c r="B208" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C208" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D208" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="209">
@@ -4036,13 +4025,13 @@
         <v>4</v>
       </c>
       <c r="B209" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C209" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D209" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="210">
@@ -4050,13 +4039,13 @@
         <v>4</v>
       </c>
       <c r="B210" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C210" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D210" t="s">
-        <v>25</v>
+        <v>233</v>
       </c>
     </row>
     <row r="211">
@@ -4064,13 +4053,13 @@
         <v>4</v>
       </c>
       <c r="B211" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C211" t="s">
         <v>30</v>
       </c>
       <c r="D211" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="212">
@@ -4078,10 +4067,10 @@
         <v>4</v>
       </c>
       <c r="B212" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C212" t="s">
-        <v>30</v>
+        <v>235</v>
       </c>
       <c r="D212" t="s">
         <v>236</v>
@@ -4092,10 +4081,10 @@
         <v>4</v>
       </c>
       <c r="B213" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C213" t="s">
-        <v>30</v>
+        <v>235</v>
       </c>
       <c r="D213" t="s">
         <v>237</v>
@@ -4106,13 +4095,13 @@
         <v>4</v>
       </c>
       <c r="B214" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="C214" t="s">
-        <v>30</v>
+        <v>239</v>
       </c>
       <c r="D214" t="s">
-        <v>238</v>
+        <v>144</v>
       </c>
     </row>
     <row r="215">
@@ -4120,21 +4109,19 @@
         <v>4</v>
       </c>
       <c r="B215" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="C215" t="s">
-        <v>30</v>
-      </c>
-      <c r="D215" t="s">
         <v>239</v>
       </c>
+      <c r="D215"/>
     </row>
     <row r="216">
       <c r="A216" t="s">
         <v>4</v>
       </c>
       <c r="B216" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="C216" t="s">
         <v>240</v>
@@ -4148,7 +4135,7 @@
         <v>4</v>
       </c>
       <c r="B217" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="C217" t="s">
         <v>240</v>
@@ -4162,13 +4149,13 @@
         <v>4</v>
       </c>
       <c r="B218" t="s">
+        <v>238</v>
+      </c>
+      <c r="C218" t="s">
+        <v>240</v>
+      </c>
+      <c r="D218" t="s">
         <v>243</v>
-      </c>
-      <c r="C218" t="s">
-        <v>244</v>
-      </c>
-      <c r="D218" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="219">
@@ -4176,25 +4163,27 @@
         <v>4</v>
       </c>
       <c r="B219" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C219" t="s">
         <v>244</v>
       </c>
-      <c r="D219"/>
+      <c r="D219" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
         <v>4</v>
       </c>
       <c r="B220" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C220" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D220" t="s">
-        <v>246</v>
+        <v>178</v>
       </c>
     </row>
     <row r="221">
@@ -4202,13 +4191,13 @@
         <v>4</v>
       </c>
       <c r="B221" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C221" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D221" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="222">
@@ -4216,13 +4205,13 @@
         <v>4</v>
       </c>
       <c r="B222" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C222" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D222" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="223">
@@ -4230,13 +4219,13 @@
         <v>4</v>
       </c>
       <c r="B223" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C223" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D223" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="224">
@@ -4244,13 +4233,13 @@
         <v>4</v>
       </c>
       <c r="B224" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C224" t="s">
         <v>249</v>
       </c>
       <c r="D224" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="225">
@@ -4258,13 +4247,13 @@
         <v>4</v>
       </c>
       <c r="B225" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C225" t="s">
         <v>249</v>
       </c>
       <c r="D225" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="226">
@@ -4272,13 +4261,13 @@
         <v>4</v>
       </c>
       <c r="B226" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C226" t="s">
         <v>249</v>
       </c>
       <c r="D226" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="227">
@@ -4286,13 +4275,13 @@
         <v>4</v>
       </c>
       <c r="B227" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C227" t="s">
         <v>249</v>
       </c>
       <c r="D227" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="228">
@@ -4300,13 +4289,13 @@
         <v>4</v>
       </c>
       <c r="B228" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C228" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D228" t="s">
-        <v>184</v>
+        <v>253</v>
       </c>
     </row>
     <row r="229">
@@ -4314,13 +4303,13 @@
         <v>4</v>
       </c>
       <c r="B229" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C229" t="s">
         <v>254</v>
       </c>
       <c r="D229" t="s">
-        <v>255</v>
+        <v>144</v>
       </c>
     </row>
     <row r="230">
@@ -4328,13 +4317,13 @@
         <v>4</v>
       </c>
       <c r="B230" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C230" t="s">
         <v>254</v>
       </c>
       <c r="D230" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="231">
@@ -4342,13 +4331,13 @@
         <v>4</v>
       </c>
       <c r="B231" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C231" t="s">
         <v>254</v>
       </c>
       <c r="D231" t="s">
-        <v>257</v>
+        <v>25</v>
       </c>
     </row>
     <row r="232">
@@ -4356,13 +4345,13 @@
         <v>4</v>
       </c>
       <c r="B232" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C232" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D232" t="s">
-        <v>258</v>
+        <v>144</v>
       </c>
     </row>
     <row r="233">
@@ -4370,13 +4359,13 @@
         <v>4</v>
       </c>
       <c r="B233" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C233" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D233" t="s">
-        <v>184</v>
+        <v>257</v>
       </c>
     </row>
     <row r="234">
@@ -4384,13 +4373,13 @@
         <v>4</v>
       </c>
       <c r="B234" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C234" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D234" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="235">
@@ -4398,13 +4387,13 @@
         <v>4</v>
       </c>
       <c r="B235" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C235" t="s">
+        <v>256</v>
+      </c>
+      <c r="D235" t="s">
         <v>259</v>
-      </c>
-      <c r="D235" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="236">
@@ -4412,13 +4401,13 @@
         <v>4</v>
       </c>
       <c r="B236" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C236" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D236" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
     </row>
     <row r="237">
@@ -4426,13 +4415,13 @@
         <v>4</v>
       </c>
       <c r="B237" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C237" t="s">
+        <v>260</v>
+      </c>
+      <c r="D237" t="s">
         <v>261</v>
-      </c>
-      <c r="D237" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="238">
@@ -4440,13 +4429,13 @@
         <v>4</v>
       </c>
       <c r="B238" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C238" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D238" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="239">
@@ -4454,13 +4443,13 @@
         <v>4</v>
       </c>
       <c r="B239" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C239" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D239" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="240">
@@ -4468,69 +4457,13 @@
         <v>4</v>
       </c>
       <c r="B240" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C240" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D240" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="s">
-        <v>4</v>
-      </c>
-      <c r="B241" t="s">
-        <v>243</v>
-      </c>
-      <c r="C241" t="s">
-        <v>265</v>
-      </c>
-      <c r="D241" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="s">
-        <v>4</v>
-      </c>
-      <c r="B242" t="s">
-        <v>243</v>
-      </c>
-      <c r="C242" t="s">
-        <v>265</v>
-      </c>
-      <c r="D242" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="s">
-        <v>4</v>
-      </c>
-      <c r="B243" t="s">
-        <v>243</v>
-      </c>
-      <c r="C243" t="s">
-        <v>265</v>
-      </c>
-      <c r="D243" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="s">
-        <v>4</v>
-      </c>
-      <c r="B244" t="s">
-        <v>243</v>
-      </c>
-      <c r="C244" t="s">
-        <v>265</v>
-      </c>
-      <c r="D244" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>